<commit_message>
Complete the expense section and fixes some ui issues
</commit_message>
<xml_diff>
--- a/Backend/Expense_Details.xlsx
+++ b/Backend/Expense_Details.xlsx
@@ -418,16 +418,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>office</v>
+        <v>https://cdn.jsdelivr.net/npm/emoji-datasource-apple/img/apple/64/1f4c8.png</v>
       </c>
       <c r="B2">
-        <v>400</v>
+        <v>10000</v>
       </c>
       <c r="C2" t="str">
-        <v>food</v>
+        <v>Trading Loss</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-04-12</v>
+        <v>2025-04-24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>